<commit_message>
Updated json file and excel file
</commit_message>
<xml_diff>
--- a/data/asciitable.xlsx
+++ b/data/asciitable.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BitaraPC\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\Repository\Web\my-ascii-table\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="299">
   <si>
     <t>&amp;#0;</t>
   </si>
@@ -876,6 +876,51 @@
   </si>
   <si>
     <t>CHARACTER</t>
+  </si>
+  <si>
+    <t>7B</t>
+  </si>
+  <si>
+    <t>&amp;#123;</t>
+  </si>
+  <si>
+    <t>{</t>
+  </si>
+  <si>
+    <t>7C</t>
+  </si>
+  <si>
+    <t>&amp;#124;</t>
+  </si>
+  <si>
+    <t>|</t>
+  </si>
+  <si>
+    <t>7D</t>
+  </si>
+  <si>
+    <t>&amp;#125;</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t>7E</t>
+  </si>
+  <si>
+    <t>&amp;#126;</t>
+  </si>
+  <si>
+    <t>~</t>
+  </si>
+  <si>
+    <t>7F</t>
+  </si>
+  <si>
+    <t>&amp;#127;</t>
+  </si>
+  <si>
+    <t>DEL</t>
   </si>
 </sst>
 </file>
@@ -1232,10 +1277,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F124"/>
+  <dimension ref="A1:F129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A119" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E129" sqref="E129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3460,7 +3505,7 @@
       </c>
       <c r="F123" s="1"/>
     </row>
-    <row r="124" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="3">
         <v>122</v>
       </c>
@@ -3477,6 +3522,96 @@
         <v>278</v>
       </c>
       <c r="F124" s="1"/>
+    </row>
+    <row r="125" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="3">
+        <v>123</v>
+      </c>
+      <c r="B125" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="C125" s="3">
+        <v>1111011</v>
+      </c>
+      <c r="D125" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="E125" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="F125" s="1"/>
+    </row>
+    <row r="126" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A126" s="3">
+        <v>124</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="C126" s="3">
+        <v>1111100</v>
+      </c>
+      <c r="D126" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="E126" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="F126" s="1"/>
+    </row>
+    <row r="127" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A127" s="3">
+        <v>125</v>
+      </c>
+      <c r="B127" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="C127" s="3">
+        <v>1111101</v>
+      </c>
+      <c r="D127" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="E127" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="F127" s="1"/>
+    </row>
+    <row r="128" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A128" s="3">
+        <v>126</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="C128" s="3">
+        <v>1111110</v>
+      </c>
+      <c r="D128" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="E128" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="F128" s="1"/>
+    </row>
+    <row r="129" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A129" s="3">
+        <v>127</v>
+      </c>
+      <c r="B129" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="C129" s="3">
+        <v>1111111</v>
+      </c>
+      <c r="D129" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="E129" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="F129" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>